<commit_message>
Updated as per discussion with Shrikant
</commit_message>
<xml_diff>
--- a/docs/requirements/MasterQueryLog_MOSIP_17Jan'19.xlsx
+++ b/docs/requirements/MasterQueryLog_MOSIP_17Jan'19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\git-repo\mosip\docs\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{61394E2E-3377-47CC-A068-92604F17E040}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5E8BDC53-F209-43B5-BF7B-203CE234B7C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3574" uniqueCount="1035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3648" uniqueCount="1053">
   <si>
     <t>MOSIP - QUERY LOG</t>
   </si>
@@ -12030,10 +12030,6 @@
 This is based on India stats which is: 30 TSPs and 280 AUAs.</t>
   </si>
   <si>
-    <t>What is the requirement wrt length of TSP ID and AUA ID? We had earlier concluded to keep it 4 digits. However please note India stats we analyzed and confirm the requirement.
-30 TSPs and 280 AUAs</t>
-  </si>
-  <si>
     <t>Email dated 29Jan'19</t>
   </si>
   <si>
@@ -12042,6 +12038,231 @@
 By default the config should be to send the notification in both languages.The Primary and Secondary language referred here is the language as configured by the admin
 The template for SMS notification and/or email notification should comprise of the content in both languages – Basically one SMS and one email notification for both languages.
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-registration:
+1. At any given point in time, MOSIP will display only two languages (Primary and Secondary) for selection by the individual
+2. These languages are driven by the admin Config 
+3. The user can choose one as primary and the other one automatically becomes the secondary. The admin sets the default primary but the user can override it, only to facilitate input of data and flow through the pre-reg. process in the preferred language
+4. Transliteration will therefore be supported for these two languages only. Data entered on the LHS will be transliterated and displayed on the RHS. Transliterated data can be updated on the RHS but will not reverse update the original data entered on the LHS
+5. MOSIP will subsequently store the data in the two languages only, along with the language code
+6. On subsequent login, if the individual has existing applications, and the individual selects the primary language to be contradictory to the language chosen during the input of data, MOSIP should consider the language choice made during current login and display the data accordingly (As data is in any case stored in both the languages)
+Registration Client:
+1. At any given point in time, MOSIP will display the demographic form in two languages only (Primary and Secondary)
+2. These languages are driven by the admin Config 
+3. Pre-reg. data download to Reg. Client: 
+a. Reg. Client will identify the data in the packet based on the language code and accordingly render it on the demographic form on the LHS or RHS (Basically, identify if the data is Primary or Secondary based on Language code associated and accordingly display it)  
+4. Transliteration will therefore be supported for these two languages only. Data entered on the LHS will be transliterated and displayed on the RHS. Transliterated data can be updated on the RHS but will not reverse update the original data entered on the LHS.
+</t>
+  </si>
+  <si>
+    <t>Email dated 30Jan'19</t>
+  </si>
+  <si>
+    <t>This needs further analysis.</t>
+  </si>
+  <si>
+    <t>Refer email dated 29Jan'19</t>
+  </si>
+  <si>
+    <t>Refer email dated 17Jan'19</t>
+  </si>
+  <si>
+    <t>Refer email dated 30Jan'19</t>
+  </si>
+  <si>
+    <t>Registration Client</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Multiple Language Support</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+What is the requirement in terms of multiple language support for Pre-registration and Registration Client?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Individual's Consent on Data Sharing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+1. Is there a requirement to seek consent of the individual during pre-registration, as individual's data is being stored and further used for UIN generation?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Individual's Consent on Data Sharing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+1. Is there a requirement for the RO to mark that the individual has provided his/her consent to store his/her data and further use for UIN generation/authentication?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>TSP ID and User Agency ID Length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+What is the requirement wrt length of TSP ID and AUA ID? We had earlier concluded to keep it 4 digits. However please note India stats we analyzed and confirm the requirement.
+30 TSPs and 280 AUAs</t>
+    </r>
+  </si>
+  <si>
+    <t>No. The system is not required to track if a new registration is for the first time or as a result of being notified to re-register. MOSIP should not maintain any link between these packets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When Reg. Client is offline, on completion of a registration, notifications cannot be triggered to the individual. In this case, the notifications should be queued and triggered to the individual whenever the Client is online. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Notifications when Reg. Client is offline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+1. How should notifications be handled, when Reg. Client is offline?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Trigger notification to additional recipients</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+1. Is it ok to have this feature of manually entering additional mobile numbers/email IDs to trigger notification to additional recipients, considering the RO can misuse this feature/data being shared through notification?</t>
+    </r>
+  </si>
+  <si>
+    <t>Yes. We should have this feature, as data being shared as part of notification essentially includes the name of the individual and RID only.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Flag to mark an individual as a “Re-registration Application”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+1. Is there a requirement to flag if a new registration is as a result of being notified to re-register due to failed packet processing?</t>
+    </r>
+  </si>
+  <si>
+    <t>Yes. On initiating a new application, before entering the demographic data, MOSIP should provide an explicit option (Recommend a pop-up with check-box to give consent) to the individual to give his/her consent for storing/utilizing the data as appropriate. This consent should be sought for every applicant.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Yes. For every registration, MOSIP should provide an option for the RO to mark an individual's consent. This should be provided on the "Preview" page. The options provided shoud be: Yes/No. If the RO marks "No" for a specific registration, this should </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> inhibit issuance of UIN for that individual. Whether the consent is marked as Yes/No should not have any impact on issuance of UIN for that individual and and MOSIP should not execute any validations in this regard during packet processing.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -21974,11 +22195,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:M233"/>
+  <dimension ref="A1:M239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A234" sqref="A234"/>
+      <pane ySplit="2" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A240" sqref="A240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -29930,7 +30151,7 @@
         <v>975</v>
       </c>
       <c r="E218" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F218" s="11" t="s">
         <v>523</v>
@@ -29943,9 +30164,15 @@
       <c r="J218" s="11" t="s">
         <v>1020</v>
       </c>
-      <c r="K218" s="8"/>
-      <c r="L218" s="8"/>
-      <c r="M218" s="11"/>
+      <c r="K218" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L218" s="9">
+        <v>43482</v>
+      </c>
+      <c r="M218" s="11" t="s">
+        <v>1038</v>
+      </c>
     </row>
     <row r="219" spans="1:13" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A219" s="8">
@@ -29961,7 +30188,7 @@
         <v>975</v>
       </c>
       <c r="E219" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F219" s="11" t="s">
         <v>523</v>
@@ -29974,9 +30201,15 @@
       <c r="J219" s="11" t="s">
         <v>1021</v>
       </c>
-      <c r="K219" s="8"/>
-      <c r="L219" s="8"/>
-      <c r="M219" s="11"/>
+      <c r="K219" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L219" s="9">
+        <v>43482</v>
+      </c>
+      <c r="M219" s="11" t="s">
+        <v>1038</v>
+      </c>
     </row>
     <row r="220" spans="1:13" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A220" s="8">
@@ -29992,7 +30225,7 @@
         <v>975</v>
       </c>
       <c r="E220" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F220" s="11" t="s">
         <v>523</v>
@@ -30005,9 +30238,15 @@
       <c r="J220" s="11" t="s">
         <v>1022</v>
       </c>
-      <c r="K220" s="8"/>
-      <c r="L220" s="8"/>
-      <c r="M220" s="11"/>
+      <c r="K220" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L220" s="9">
+        <v>43482</v>
+      </c>
+      <c r="M220" s="11" t="s">
+        <v>1038</v>
+      </c>
     </row>
     <row r="221" spans="1:13" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A221" s="8">
@@ -30023,7 +30262,7 @@
         <v>975</v>
       </c>
       <c r="E221" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F221" s="11" t="s">
         <v>523</v>
@@ -30036,9 +30275,15 @@
       <c r="J221" s="11" t="s">
         <v>1029</v>
       </c>
-      <c r="K221" s="8"/>
-      <c r="L221" s="8"/>
-      <c r="M221" s="11"/>
+      <c r="K221" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L221" s="9">
+        <v>43482</v>
+      </c>
+      <c r="M221" s="11" t="s">
+        <v>1038</v>
+      </c>
     </row>
     <row r="222" spans="1:13" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A222" s="8">
@@ -30054,7 +30299,7 @@
         <v>975</v>
       </c>
       <c r="E222" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F222" s="11" t="s">
         <v>523</v>
@@ -30067,9 +30312,15 @@
       <c r="J222" s="11" t="s">
         <v>1023</v>
       </c>
-      <c r="K222" s="8"/>
-      <c r="L222" s="8"/>
-      <c r="M222" s="11"/>
+      <c r="K222" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L222" s="9">
+        <v>43482</v>
+      </c>
+      <c r="M222" s="11" t="s">
+        <v>1038</v>
+      </c>
     </row>
     <row r="223" spans="1:13" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A223" s="8">
@@ -30085,7 +30336,7 @@
         <v>975</v>
       </c>
       <c r="E223" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F223" s="11" t="s">
         <v>523</v>
@@ -30098,9 +30349,15 @@
       <c r="J223" s="11" t="s">
         <v>1024</v>
       </c>
-      <c r="K223" s="8"/>
-      <c r="L223" s="8"/>
-      <c r="M223" s="11"/>
+      <c r="K223" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L223" s="9">
+        <v>43482</v>
+      </c>
+      <c r="M223" s="11" t="s">
+        <v>1038</v>
+      </c>
     </row>
     <row r="224" spans="1:13" ht="195.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="8">
@@ -30116,7 +30373,7 @@
         <v>975</v>
       </c>
       <c r="E224" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F224" s="11" t="s">
         <v>523</v>
@@ -30129,9 +30386,15 @@
       <c r="J224" s="11" t="s">
         <v>1025</v>
       </c>
-      <c r="K224" s="8"/>
-      <c r="L224" s="8"/>
-      <c r="M224" s="11"/>
+      <c r="K224" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L224" s="9">
+        <v>43482</v>
+      </c>
+      <c r="M224" s="11" t="s">
+        <v>1038</v>
+      </c>
     </row>
     <row r="225" spans="1:13" ht="199.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="63">
@@ -30186,7 +30449,7 @@
         <v>217</v>
       </c>
       <c r="E226" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F226" s="11" t="s">
         <v>779</v>
@@ -30197,11 +30460,17 @@
       <c r="H226" s="8"/>
       <c r="I226" s="12"/>
       <c r="J226" s="11" t="s">
-        <v>1034</v>
-      </c>
-      <c r="K226" s="8"/>
-      <c r="L226" s="8"/>
-      <c r="M226" s="11"/>
+        <v>1033</v>
+      </c>
+      <c r="K226" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="L226" s="9">
+        <v>43494</v>
+      </c>
+      <c r="M226" s="11" t="s">
+        <v>1037</v>
+      </c>
     </row>
     <row r="227" spans="1:13" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A227" s="8">
@@ -30217,7 +30486,7 @@
         <v>217</v>
       </c>
       <c r="E227" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F227" s="11" t="s">
         <v>1012</v>
@@ -30228,11 +30497,17 @@
       <c r="H227" s="8"/>
       <c r="I227" s="12"/>
       <c r="J227" s="11" t="s">
-        <v>1034</v>
-      </c>
-      <c r="K227" s="8"/>
-      <c r="L227" s="8"/>
-      <c r="M227" s="11"/>
+        <v>1033</v>
+      </c>
+      <c r="K227" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="L227" s="9">
+        <v>43494</v>
+      </c>
+      <c r="M227" s="11" t="s">
+        <v>1037</v>
+      </c>
     </row>
     <row r="228" spans="1:13" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A228" s="8">
@@ -30248,7 +30523,7 @@
         <v>217</v>
       </c>
       <c r="E228" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F228" s="11" t="s">
         <v>523</v>
@@ -30259,11 +30534,17 @@
       <c r="H228" s="8"/>
       <c r="I228" s="12"/>
       <c r="J228" s="11" t="s">
-        <v>1034</v>
-      </c>
-      <c r="K228" s="8"/>
-      <c r="L228" s="8"/>
-      <c r="M228" s="11"/>
+        <v>1033</v>
+      </c>
+      <c r="K228" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="L228" s="9">
+        <v>43494</v>
+      </c>
+      <c r="M228" s="11" t="s">
+        <v>1037</v>
+      </c>
     </row>
     <row r="229" spans="1:13" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A229" s="8">
@@ -30279,7 +30560,7 @@
         <v>986</v>
       </c>
       <c r="E229" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F229" s="11" t="s">
         <v>654</v>
@@ -30292,9 +30573,15 @@
       <c r="J229" s="11" t="s">
         <v>1026</v>
       </c>
-      <c r="K229" s="8"/>
-      <c r="L229" s="8"/>
-      <c r="M229" s="11"/>
+      <c r="K229" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L229" s="9">
+        <v>43482</v>
+      </c>
+      <c r="M229" s="11" t="s">
+        <v>1038</v>
+      </c>
     </row>
     <row r="230" spans="1:13" ht="228" x14ac:dyDescent="0.25">
       <c r="A230" s="8">
@@ -30310,7 +30597,7 @@
         <v>986</v>
       </c>
       <c r="E230" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F230" s="11" t="s">
         <v>654</v>
@@ -30323,9 +30610,15 @@
       <c r="J230" s="11" t="s">
         <v>1027</v>
       </c>
-      <c r="K230" s="8"/>
-      <c r="L230" s="8"/>
-      <c r="M230" s="11"/>
+      <c r="K230" s="8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L230" s="9">
+        <v>43482</v>
+      </c>
+      <c r="M230" s="11" t="s">
+        <v>1038</v>
+      </c>
     </row>
     <row r="231" spans="1:13" ht="85.5" x14ac:dyDescent="0.25">
       <c r="A231" s="8">
@@ -30380,7 +30673,9 @@
       <c r="G232" s="45" t="s">
         <v>1030</v>
       </c>
-      <c r="J232" s="11"/>
+      <c r="J232" s="11" t="s">
+        <v>1036</v>
+      </c>
       <c r="K232" s="8"/>
       <c r="L232" s="8"/>
       <c r="M232" s="11"/>
@@ -30396,23 +30691,237 @@
         <v>39</v>
       </c>
       <c r="D233" s="11" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="E233" s="11" t="s">
-        <v>1019</v>
+        <v>24</v>
       </c>
       <c r="F233" s="11" t="s">
         <v>776</v>
       </c>
       <c r="G233" s="11" t="s">
-        <v>1032</v>
+        <v>1044</v>
       </c>
       <c r="J233" s="11" t="s">
         <v>1031</v>
       </c>
-      <c r="K233" s="8"/>
-      <c r="L233" s="8"/>
+      <c r="K233" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="L233" s="9">
+        <v>43494</v>
+      </c>
       <c r="M233" s="11"/>
+    </row>
+    <row r="234" spans="1:13" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="8">
+        <v>232</v>
+      </c>
+      <c r="B234" s="9">
+        <v>43495</v>
+      </c>
+      <c r="C234" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D234" s="11" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E234" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F234" s="11" t="s">
+        <v>776</v>
+      </c>
+      <c r="G234" s="11" t="s">
+        <v>1041</v>
+      </c>
+      <c r="J234" s="11" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K234" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="L234" s="9">
+        <v>43495</v>
+      </c>
+      <c r="M234" s="11" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A235" s="8">
+        <v>233</v>
+      </c>
+      <c r="B235" s="9">
+        <v>43495</v>
+      </c>
+      <c r="C235" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D235" s="11" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E235" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F235" s="11" t="s">
+        <v>1012</v>
+      </c>
+      <c r="G235" s="11" t="s">
+        <v>1042</v>
+      </c>
+      <c r="J235" s="11" t="s">
+        <v>1051</v>
+      </c>
+      <c r="K235" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="L235" s="9">
+        <v>43495</v>
+      </c>
+      <c r="M235" s="11" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A236" s="8">
+        <v>234</v>
+      </c>
+      <c r="B236" s="9">
+        <v>43495</v>
+      </c>
+      <c r="C236" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D236" s="11" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E236" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F236" s="11" t="s">
+        <v>1040</v>
+      </c>
+      <c r="G236" s="11" t="s">
+        <v>1043</v>
+      </c>
+      <c r="J236" s="11" t="s">
+        <v>1052</v>
+      </c>
+      <c r="K236" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="L236" s="9">
+        <v>43495</v>
+      </c>
+      <c r="M236" s="11" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" ht="57" x14ac:dyDescent="0.25">
+      <c r="A237" s="8">
+        <v>235</v>
+      </c>
+      <c r="B237" s="9">
+        <v>43495</v>
+      </c>
+      <c r="C237" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D237" s="11" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E237" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F237" s="11" t="s">
+        <v>1040</v>
+      </c>
+      <c r="G237" s="11" t="s">
+        <v>1050</v>
+      </c>
+      <c r="J237" s="11" t="s">
+        <v>1045</v>
+      </c>
+      <c r="K237" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="L237" s="9">
+        <v>43495</v>
+      </c>
+      <c r="M237" s="11" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" ht="57" x14ac:dyDescent="0.25">
+      <c r="A238" s="8">
+        <v>236</v>
+      </c>
+      <c r="B238" s="9">
+        <v>43495</v>
+      </c>
+      <c r="C238" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D238" s="11" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E238" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F238" s="11" t="s">
+        <v>1040</v>
+      </c>
+      <c r="G238" s="11" t="s">
+        <v>1047</v>
+      </c>
+      <c r="J238" s="11" t="s">
+        <v>1046</v>
+      </c>
+      <c r="K238" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="L238" s="9">
+        <v>43495</v>
+      </c>
+      <c r="M238" s="11" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="A239" s="8">
+        <v>237</v>
+      </c>
+      <c r="B239" s="9">
+        <v>43495</v>
+      </c>
+      <c r="C239" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D239" s="11" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E239" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F239" s="11" t="s">
+        <v>1040</v>
+      </c>
+      <c r="G239" s="11" t="s">
+        <v>1048</v>
+      </c>
+      <c r="J239" s="11" t="s">
+        <v>1049</v>
+      </c>
+      <c r="K239" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="L239" s="9">
+        <v>43495</v>
+      </c>
+      <c r="M239" s="11" t="s">
+        <v>1039</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:M231" xr:uid="{00000000-0009-0000-0000-000001000000}">
@@ -30656,6 +31165,41 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
+    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -30862,56 +31406,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ProjectIGName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectIGName>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <ProjectAccountName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">Mindtree</ProjectAccountName>
-    <ProjectName xmlns="fd9ad297-cc8c-4afc-b828-e13c9647a5fa">MOSIP</ProjectName>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F1DD169-1613-4852-8D49-4C3CB1FDBF80}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -30934,9 +31432,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F1DD169-1613-4852-8D49-4C3CB1FDBF80}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="fd9ad297-cc8c-4afc-b828-e13c9647a5fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added 254 and 255 on UIN Update and VID
</commit_message>
<xml_diff>
--- a/docs/requirements/MasterQueryLog_MOSIP_17Jan'19.xlsx
+++ b/docs/requirements/MasterQueryLog_MOSIP_17Jan'19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1002694\Documents\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC82220A-70BF-442B-B955-06D0DF44739A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B13339-99B9-4CF0-8824-FE64047EAFB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8532" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3760" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3765" uniqueCount="1099">
   <si>
     <t>MOSIP - QUERY LOG</t>
   </si>
@@ -12688,6 +12688,30 @@
 (ii) the resident might no longer have access to the old mobile number.
 The user will not be able to proceed further. A similar issue exists for change of email ID as well.
 Should we therefore mandate 'Biometrics' as the mode of authentication for all updates made through client?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>Virtual ID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>:
+1. UIN Update: Should we support entry of VIN (also called VID) instead of the UIN?
+2. Lost UIN: Should we support entry of VIN as a way to retrieve the UIN?
+3. VIN Management: Should we support generation / revocation / retrieval of VIN?</t>
     </r>
   </si>
 </sst>
@@ -22620,11 +22644,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M256"/>
+  <dimension ref="A1:M257"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C261" sqref="C261"/>
+      <selection pane="bottomLeft" activeCell="G258" sqref="G258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.21875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -31918,6 +31942,35 @@
       <c r="K256" s="8"/>
       <c r="L256" s="9"/>
       <c r="M256" s="11"/>
+    </row>
+    <row r="257" spans="1:13" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A257" s="8">
+        <v>255</v>
+      </c>
+      <c r="B257" s="9">
+        <v>43537</v>
+      </c>
+      <c r="C257" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D257" s="11" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E257" s="11" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F257" s="11" t="s">
+        <v>1039</v>
+      </c>
+      <c r="G257" s="11" t="s">
+        <v>1098</v>
+      </c>
+      <c r="H257" s="8"/>
+      <c r="I257" s="12"/>
+      <c r="J257" s="11"/>
+      <c r="K257" s="8"/>
+      <c r="L257" s="9"/>
+      <c r="M257" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:M251" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
@@ -32155,15 +32208,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -32370,6 +32414,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -32397,14 +32450,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F1DD169-1613-4852-8D49-4C3CB1FDBF80}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32419,6 +32464,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>